<commit_message>
adding column to data if the response was a percent
</commit_message>
<xml_diff>
--- a/Data/Old data/Full_data_ML3.xlsx
+++ b/Data/Old data/Full_data_ML3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/losialagisz/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinmacartney/Documents/EE_stress_MA/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4844A1B-B19D-924A-9CEC-5F5F18F8864E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F53926-D359-9D41-AE58-17E29CABF39C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="40580" windowHeight="23040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - Full_data" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -247,7 +247,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="488">
   <si>
     <t>Study_ID</t>
   </si>
@@ -1615,13 +1615,109 @@
   </si>
   <si>
     <t>shock</t>
+  </si>
+  <si>
+    <t>7.12, 12.18</t>
+  </si>
+  <si>
+    <t>9.12, 10.65</t>
+  </si>
+  <si>
+    <t>1.53, 4.05</t>
+  </si>
+  <si>
+    <t>3.55, 10.65</t>
+  </si>
+  <si>
+    <t>16.22, 11.16</t>
+  </si>
+  <si>
+    <t>21.8, 3.55</t>
+  </si>
+  <si>
+    <t>6.09, 8.62</t>
+  </si>
+  <si>
+    <t>9.63, 3.04</t>
+  </si>
+  <si>
+    <t>9.36,  8.19</t>
+  </si>
+  <si>
+    <t>14.04, 9.35</t>
+  </si>
+  <si>
+    <t>3.5, 10.52</t>
+  </si>
+  <si>
+    <t>8.19, 10.53</t>
+  </si>
+  <si>
+    <t>10.53, 12.86</t>
+  </si>
+  <si>
+    <t>9.36, 8.19</t>
+  </si>
+  <si>
+    <t>5.85, 10.52</t>
+  </si>
+  <si>
+    <t>10.53, 8.19</t>
+  </si>
+  <si>
+    <t>20.7,  11.15</t>
+  </si>
+  <si>
+    <t>15.93, 9.55</t>
+  </si>
+  <si>
+    <t>7.96,  6.37</t>
+  </si>
+  <si>
+    <t>23.88, 15.93</t>
+  </si>
+  <si>
+    <t>12.74 , 6.37</t>
+  </si>
+  <si>
+    <t>23.88, 15.92</t>
+  </si>
+  <si>
+    <t>12.74, 6.37</t>
+  </si>
+  <si>
+    <t>6.37, 7.96</t>
+  </si>
+  <si>
+    <t>10.34, 8. 42</t>
+  </si>
+  <si>
+    <t>17.6, 11.11</t>
+  </si>
+  <si>
+    <t>10.72, 12.25</t>
+  </si>
+  <si>
+    <t>8.42, 9.57</t>
+  </si>
+  <si>
+    <t>1.73, 1.1</t>
+  </si>
+  <si>
+    <t>1.9, 1.21</t>
+  </si>
+  <si>
+    <t>2.59, 1.26</t>
+  </si>
+  <si>
+    <t>2.24, 1.04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1629,6 +1725,12 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -1921,7 +2023,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2046,6 +2148,27 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -10037,7 +10160,173 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C2E2E2D7-C779-FE42-94F2-12B0B7E709E0}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8778D12E-7CCE-A247-96E6-0CEEC95E66B0}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="L36:M42" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="75">
+    <pivotField dataField="1" showAll="0">
+      <items count="33">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="27"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Study_ID" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C2E2E2D7-C779-FE42-94F2-12B0B7E709E0}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B33" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="75">
     <pivotField showAll="0">
@@ -10411,8 +10700,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E2FEF28A-B3FE-984A-8BCE-ED2844012400}" name="PivotTable3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E2FEF28A-B3FE-984A-8BCE-ED2844012400}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A46:G52" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="75">
     <pivotField showAll="0"/>
@@ -10667,8 +10956,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F48DB254-D1C8-C949-A25A-C9C26EF05E66}" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F48DB254-D1C8-C949-A25A-C9C26EF05E66}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A36:E43" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="75">
     <pivotField showAll="0"/>
@@ -10906,172 +11195,6 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Count of ES_ID" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8778D12E-7CCE-A247-96E6-0CEEC95E66B0}" name="PivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="L36:M42" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="75">
-    <pivotField dataField="1" showAll="0">
-      <items count="33">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="27"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Study_ID" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -12240,8 +12363,12 @@
   </sheetPr>
   <dimension ref="A1:BW97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N91" workbookViewId="0">
-      <selection activeCell="Z114" sqref="Z114"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="AY84" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="BJ97" sqref="BJ97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -12285,7 +12412,7 @@
     <col min="38" max="38" width="5.83203125" style="1" customWidth="1"/>
     <col min="39" max="39" width="9.1640625" style="1" customWidth="1"/>
     <col min="40" max="40" width="10.6640625" style="1" customWidth="1"/>
-    <col min="41" max="41" width="11.1640625" style="1" customWidth="1"/>
+    <col min="41" max="41" width="11.1640625" style="46" customWidth="1"/>
     <col min="42" max="42" width="7" style="1" customWidth="1"/>
     <col min="43" max="44" width="16.1640625" style="1" customWidth="1"/>
     <col min="45" max="45" width="5.6640625" style="1" customWidth="1"/>
@@ -12442,7 +12569,7 @@
       <c r="AN1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AO1" s="43" t="s">
         <v>40</v>
       </c>
       <c r="AP1" s="2" t="s">
@@ -12661,7 +12788,7 @@
         <v>10.5</v>
       </c>
       <c r="AN2" s="7"/>
-      <c r="AO2" s="5">
+      <c r="AO2" s="44">
         <v>4.46</v>
       </c>
       <c r="AP2" s="5">
@@ -12850,7 +12977,7 @@
         <v>191.8</v>
       </c>
       <c r="AN3" s="12"/>
-      <c r="AO3" s="10">
+      <c r="AO3" s="45">
         <v>69.98</v>
       </c>
       <c r="AP3" s="10">
@@ -13039,7 +13166,7 @@
         <v>17.55</v>
       </c>
       <c r="AN4" s="12"/>
-      <c r="AO4" s="10">
+      <c r="AO4" s="45">
         <v>3.1</v>
       </c>
       <c r="AP4" s="10">
@@ -13230,7 +13357,7 @@
         <v>3.37</v>
       </c>
       <c r="AN5" s="12"/>
-      <c r="AO5" s="10">
+      <c r="AO5" s="45">
         <v>0.85</v>
       </c>
       <c r="AP5" s="10">
@@ -13415,7 +13542,7 @@
         <v>64.83</v>
       </c>
       <c r="AN6" s="12"/>
-      <c r="AO6" s="10">
+      <c r="AO6" s="45">
         <v>18.350000000000001</v>
       </c>
       <c r="AP6" s="10">
@@ -13600,7 +13727,7 @@
         <v>74.27</v>
       </c>
       <c r="AN7" s="12"/>
-      <c r="AO7" s="10">
+      <c r="AO7" s="45">
         <v>13.99</v>
       </c>
       <c r="AP7" s="10">
@@ -13783,7 +13910,7 @@
         <v>38.22</v>
       </c>
       <c r="AN8" s="12"/>
-      <c r="AO8" s="10">
+      <c r="AO8" s="45">
         <v>5.44</v>
       </c>
       <c r="AP8" s="10">
@@ -13962,7 +14089,7 @@
         <v>43.04</v>
       </c>
       <c r="AN9" s="12"/>
-      <c r="AO9" s="10">
+      <c r="AO9" s="45">
         <v>9.77</v>
       </c>
       <c r="AP9" s="10">
@@ -14147,7 +14274,7 @@
         <v>18.690000000000001</v>
       </c>
       <c r="AN10" s="12"/>
-      <c r="AO10" s="10">
+      <c r="AO10" s="45">
         <v>5.8548441479999997</v>
       </c>
       <c r="AP10" s="10">
@@ -14334,7 +14461,7 @@
         <v>52.94</v>
       </c>
       <c r="AN11" s="12"/>
-      <c r="AO11" s="10">
+      <c r="AO11" s="45">
         <v>38.494893169999997</v>
       </c>
       <c r="AP11" s="10">
@@ -14517,7 +14644,7 @@
         <v>33</v>
       </c>
       <c r="AN12" s="12"/>
-      <c r="AO12" s="10">
+      <c r="AO12" s="45">
         <v>9.9863506849999997</v>
       </c>
       <c r="AP12" s="10">
@@ -14698,7 +14825,7 @@
         <v>28.5</v>
       </c>
       <c r="AN13" s="12"/>
-      <c r="AO13" s="10">
+      <c r="AO13" s="45">
         <v>22.5</v>
       </c>
       <c r="AP13" s="10">
@@ -14881,7 +15008,7 @@
         <v>62.3</v>
       </c>
       <c r="AN14" s="12"/>
-      <c r="AO14" s="10">
+      <c r="AO14" s="45">
         <v>26.97</v>
       </c>
       <c r="AP14" s="10">
@@ -15064,7 +15191,7 @@
         <v>56.59</v>
       </c>
       <c r="AN15" s="12"/>
-      <c r="AO15" s="10">
+      <c r="AO15" s="45">
         <v>10.17</v>
       </c>
       <c r="AP15" s="10">
@@ -15247,7 +15374,7 @@
         <v>84.75</v>
       </c>
       <c r="AN16" s="12"/>
-      <c r="AO16" s="10">
+      <c r="AO16" s="45">
         <v>110.62</v>
       </c>
       <c r="AP16" s="10">
@@ -15428,7 +15555,7 @@
         <v>149.33000000000001</v>
       </c>
       <c r="AN17" s="12"/>
-      <c r="AO17" s="10">
+      <c r="AO17" s="45">
         <v>170.16</v>
       </c>
       <c r="AP17" s="10">
@@ -15609,7 +15736,7 @@
         <v>13.82</v>
       </c>
       <c r="AN18" s="12"/>
-      <c r="AO18" s="10">
+      <c r="AO18" s="45">
         <v>5.46</v>
       </c>
       <c r="AP18" s="10">
@@ -15790,7 +15917,7 @@
         <v>17.45</v>
       </c>
       <c r="AN19" s="12"/>
-      <c r="AO19" s="10">
+      <c r="AO19" s="45">
         <v>12</v>
       </c>
       <c r="AP19" s="10">
@@ -15971,7 +16098,7 @@
         <v>30.3</v>
       </c>
       <c r="AN20" s="12"/>
-      <c r="AO20" s="10">
+      <c r="AO20" s="45">
         <v>18.18</v>
       </c>
       <c r="AP20" s="10">
@@ -16150,7 +16277,7 @@
         <v>48.28</v>
       </c>
       <c r="AN21" s="12"/>
-      <c r="AO21" s="10">
+      <c r="AO21" s="45">
         <v>27.6</v>
       </c>
       <c r="AP21" s="10">
@@ -16331,7 +16458,7 @@
         <v>14.5</v>
       </c>
       <c r="AN22" s="12"/>
-      <c r="AO22" s="10">
+      <c r="AO22" s="45">
         <v>16.18</v>
       </c>
       <c r="AP22" s="10">
@@ -16512,7 +16639,7 @@
         <v>45.57</v>
       </c>
       <c r="AN23" s="12"/>
-      <c r="AO23" s="10">
+      <c r="AO23" s="45">
         <v>22.04</v>
       </c>
       <c r="AP23" s="10">
@@ -16691,7 +16818,7 @@
         <v>17.329999999999998</v>
       </c>
       <c r="AN24" s="12"/>
-      <c r="AO24" s="10">
+      <c r="AO24" s="45">
         <v>13.04</v>
       </c>
       <c r="AP24" s="10">
@@ -16874,7 +17001,7 @@
         <v>11.93</v>
       </c>
       <c r="AN25" s="12"/>
-      <c r="AO25" s="10">
+      <c r="AO25" s="45">
         <v>6.48</v>
       </c>
       <c r="AP25" s="10">
@@ -17057,7 +17184,7 @@
         <v>10.050000000000001</v>
       </c>
       <c r="AN26" s="12"/>
-      <c r="AO26" s="10">
+      <c r="AO26" s="45">
         <v>1.72</v>
       </c>
       <c r="AP26" s="10">
@@ -17238,7 +17365,7 @@
         <v>9.6</v>
       </c>
       <c r="AN27" s="12"/>
-      <c r="AO27" s="10">
+      <c r="AO27" s="45">
         <v>2.54</v>
       </c>
       <c r="AP27" s="10">
@@ -17416,14 +17543,14 @@
         <v>6</v>
       </c>
       <c r="AM28" s="10">
-        <v>75.62</v>
+        <v>84.69</v>
       </c>
       <c r="AN28" s="12"/>
-      <c r="AO28" s="10">
-        <v>30.23</v>
-      </c>
-      <c r="AP28" s="10">
-        <v>12.34</v>
+      <c r="AO28" s="47">
+        <v>25.960570000000001</v>
+      </c>
+      <c r="AP28" s="42" t="s">
+        <v>456</v>
       </c>
       <c r="AQ28" s="12"/>
       <c r="AR28" s="12"/>
@@ -17431,14 +17558,14 @@
         <v>6</v>
       </c>
       <c r="AT28" s="10">
-        <v>102.37</v>
+        <v>60.35</v>
       </c>
       <c r="AU28" s="12"/>
-      <c r="AV28" s="10">
-        <v>26.45</v>
-      </c>
-      <c r="AW28" s="10">
-        <v>10.8</v>
+      <c r="AV28" s="42">
+        <v>24.429770000000001</v>
+      </c>
+      <c r="AW28" s="42" t="s">
+        <v>457</v>
       </c>
       <c r="AX28" s="12"/>
       <c r="AY28" s="12"/>
@@ -17446,14 +17573,14 @@
         <v>6</v>
       </c>
       <c r="BA28" s="10">
-        <v>74.59</v>
+        <v>54.76</v>
       </c>
       <c r="BB28" s="12"/>
-      <c r="BC28" s="10">
-        <v>12.59</v>
-      </c>
-      <c r="BD28" s="10">
-        <v>5.14</v>
+      <c r="BC28" s="42">
+        <v>8.6764849999999996</v>
+      </c>
+      <c r="BD28" s="42" t="s">
+        <v>458</v>
       </c>
       <c r="BE28" s="12"/>
       <c r="BF28" s="12"/>
@@ -17461,14 +17588,14 @@
         <v>6</v>
       </c>
       <c r="BH28" s="10">
-        <v>107</v>
+        <v>43.61</v>
       </c>
       <c r="BI28" s="12"/>
-      <c r="BJ28" s="10">
-        <v>23.93</v>
-      </c>
-      <c r="BK28" s="10">
-        <v>9.77</v>
+      <c r="BJ28" s="42">
+        <v>23.006630000000001</v>
+      </c>
+      <c r="BK28" s="42" t="s">
+        <v>459</v>
       </c>
       <c r="BL28" s="12"/>
       <c r="BM28" s="12"/>
@@ -17595,14 +17722,14 @@
         <v>6</v>
       </c>
       <c r="AM29" s="10">
-        <v>111.11</v>
+        <v>53.25</v>
       </c>
       <c r="AN29" s="12"/>
-      <c r="AO29" s="10">
-        <v>26.45</v>
-      </c>
-      <c r="AP29" s="10">
-        <v>10.8</v>
+      <c r="AO29" s="47">
+        <v>35.20955</v>
+      </c>
+      <c r="AP29" s="42" t="s">
+        <v>460</v>
       </c>
       <c r="AQ29" s="12"/>
       <c r="AR29" s="12"/>
@@ -17610,14 +17737,14 @@
         <v>6</v>
       </c>
       <c r="AT29" s="10">
-        <v>96.19</v>
+        <v>75.05</v>
       </c>
       <c r="AU29" s="12"/>
-      <c r="AV29" s="10">
-        <v>8.82</v>
-      </c>
-      <c r="AW29" s="10">
-        <v>3.6</v>
+      <c r="AV29" s="42">
+        <v>49.625749999999996</v>
+      </c>
+      <c r="AW29" s="42" t="s">
+        <v>461</v>
       </c>
       <c r="AX29" s="12"/>
       <c r="AY29" s="12"/>
@@ -17625,14 +17752,14 @@
         <v>6</v>
       </c>
       <c r="BA29" s="10">
-        <v>109.57</v>
+        <v>23.83</v>
       </c>
       <c r="BB29" s="12"/>
-      <c r="BC29" s="10">
-        <v>21.41</v>
-      </c>
-      <c r="BD29" s="10">
-        <v>8.74</v>
+      <c r="BC29" s="42">
+        <v>18.798410000000001</v>
+      </c>
+      <c r="BD29" s="42" t="s">
+        <v>462</v>
       </c>
       <c r="BE29" s="12"/>
       <c r="BF29" s="12"/>
@@ -17640,14 +17767,14 @@
         <v>6</v>
       </c>
       <c r="BH29" s="10">
-        <v>80.760000000000005</v>
+        <v>45.13</v>
       </c>
       <c r="BI29" s="12"/>
-      <c r="BJ29" s="10">
-        <v>8.82</v>
-      </c>
-      <c r="BK29" s="10">
-        <v>3.6</v>
+      <c r="BJ29" s="42">
+        <v>20.88588</v>
+      </c>
+      <c r="BK29" s="42" t="s">
+        <v>463</v>
       </c>
       <c r="BL29" s="12"/>
       <c r="BM29" s="12"/>
@@ -17777,7 +17904,7 @@
         <v>33.25</v>
       </c>
       <c r="AN30" s="12"/>
-      <c r="AO30" s="10">
+      <c r="AO30" s="45">
         <v>15.92</v>
       </c>
       <c r="AP30" s="10">
@@ -17954,7 +18081,7 @@
         <v>35.25</v>
       </c>
       <c r="AN31" s="12"/>
-      <c r="AO31" s="10">
+      <c r="AO31" s="45">
         <v>7.96</v>
       </c>
       <c r="AP31" s="10">
@@ -18129,7 +18256,7 @@
         <v>28.95</v>
       </c>
       <c r="AN32" s="12"/>
-      <c r="AO32" s="10">
+      <c r="AO32" s="45">
         <v>3.95</v>
       </c>
       <c r="AP32" s="12"/>
@@ -18296,7 +18423,7 @@
         <v>62.98</v>
       </c>
       <c r="AN33" s="12"/>
-      <c r="AO33" s="10">
+      <c r="AO33" s="45">
         <v>4.8099999999999996</v>
       </c>
       <c r="AP33" s="12"/>
@@ -18463,7 +18590,7 @@
         <v>12.47</v>
       </c>
       <c r="AN34" s="12"/>
-      <c r="AO34" s="10">
+      <c r="AO34" s="45">
         <v>7.45</v>
       </c>
       <c r="AP34" s="10">
@@ -18638,7 +18765,7 @@
         <v>12.65</v>
       </c>
       <c r="AN35" s="12"/>
-      <c r="AO35" s="10">
+      <c r="AO35" s="45">
         <v>5.12</v>
       </c>
       <c r="AP35" s="10">
@@ -18815,7 +18942,7 @@
         <v>19.690000000000001</v>
       </c>
       <c r="AN36" s="12"/>
-      <c r="AO36" s="10">
+      <c r="AO36" s="45">
         <v>1.8</v>
       </c>
       <c r="AP36" s="10">
@@ -18992,7 +19119,7 @@
         <v>18.34</v>
       </c>
       <c r="AN37" s="12"/>
-      <c r="AO37" s="10">
+      <c r="AO37" s="45">
         <v>9.69</v>
       </c>
       <c r="AP37" s="12"/>
@@ -19169,7 +19296,7 @@
         <v>18.66</v>
       </c>
       <c r="AN38" s="12"/>
-      <c r="AO38" s="10">
+      <c r="AO38" s="45">
         <v>9.86</v>
       </c>
       <c r="AP38" s="12"/>
@@ -19346,7 +19473,7 @@
         <v>17.28</v>
       </c>
       <c r="AN39" s="12"/>
-      <c r="AO39" s="10">
+      <c r="AO39" s="45">
         <v>10.82</v>
       </c>
       <c r="AP39" s="12"/>
@@ -19523,7 +19650,7 @@
         <v>15.39</v>
       </c>
       <c r="AN40" s="12"/>
-      <c r="AO40" s="10">
+      <c r="AO40" s="45">
         <v>12.96</v>
       </c>
       <c r="AP40" s="12"/>
@@ -19704,7 +19831,7 @@
       <c r="AN41" s="10">
         <v>3.05</v>
       </c>
-      <c r="AO41" s="10">
+      <c r="AO41" s="45">
         <v>1.92</v>
       </c>
       <c r="AP41" s="12"/>
@@ -19903,7 +20030,7 @@
       <c r="AN42" s="10">
         <v>91.19</v>
       </c>
-      <c r="AO42" s="10">
+      <c r="AO42" s="45">
         <v>19.96</v>
       </c>
       <c r="AP42" s="12"/>
@@ -20102,7 +20229,7 @@
       <c r="AN43" s="10">
         <v>9.11</v>
       </c>
-      <c r="AO43" s="10">
+      <c r="AO43" s="45">
         <v>3.28</v>
       </c>
       <c r="AP43" s="12"/>
@@ -20299,7 +20426,7 @@
       <c r="AN44" s="10">
         <v>22.03</v>
       </c>
-      <c r="AO44" s="10">
+      <c r="AO44" s="45">
         <v>1.1399999999999999</v>
       </c>
       <c r="AP44" s="12"/>
@@ -20496,7 +20623,7 @@
       <c r="AN45" s="10">
         <v>18.059999999999999</v>
       </c>
-      <c r="AO45" s="10">
+      <c r="AO45" s="45">
         <v>3.05</v>
       </c>
       <c r="AP45" s="12"/>
@@ -20693,7 +20820,7 @@
       <c r="AN46" s="10">
         <v>412.94</v>
       </c>
-      <c r="AO46" s="10">
+      <c r="AO46" s="45">
         <v>188.24</v>
       </c>
       <c r="AP46" s="12"/>
@@ -20890,7 +21017,7 @@
       <c r="AN47" s="10">
         <v>77.39</v>
       </c>
-      <c r="AO47" s="10">
+      <c r="AO47" s="45">
         <v>18.61</v>
       </c>
       <c r="AP47" s="12"/>
@@ -21085,7 +21212,7 @@
         <v>66.91</v>
       </c>
       <c r="AN48" s="12"/>
-      <c r="AO48" s="10">
+      <c r="AO48" s="45">
         <v>17.170000000000002</v>
       </c>
       <c r="AP48" s="10">
@@ -21264,7 +21391,7 @@
         <v>12.67</v>
       </c>
       <c r="AN49" s="12"/>
-      <c r="AO49" s="10">
+      <c r="AO49" s="45">
         <v>6.8</v>
       </c>
       <c r="AP49" s="10">
@@ -21441,7 +21568,7 @@
         <v>23.43</v>
       </c>
       <c r="AN50" s="12"/>
-      <c r="AO50" s="10">
+      <c r="AO50" s="45">
         <v>5.28</v>
       </c>
       <c r="AP50" s="10">
@@ -21618,7 +21745,7 @@
         <v>3.3</v>
       </c>
       <c r="AN51" s="12"/>
-      <c r="AO51" s="10">
+      <c r="AO51" s="45">
         <v>1.45</v>
       </c>
       <c r="AP51" s="10">
@@ -21799,7 +21926,7 @@
         <v>1.48</v>
       </c>
       <c r="AN52" s="12"/>
-      <c r="AO52" s="10">
+      <c r="AO52" s="45">
         <v>0.81</v>
       </c>
       <c r="AP52" s="10">
@@ -21980,7 +22107,7 @@
         <v>2.02</v>
       </c>
       <c r="AN53" s="12"/>
-      <c r="AO53" s="10">
+      <c r="AO53" s="45">
         <v>1.65</v>
       </c>
       <c r="AP53" s="10">
@@ -22157,7 +22284,7 @@
         <v>20.62</v>
       </c>
       <c r="AN54" s="12"/>
-      <c r="AO54" s="10">
+      <c r="AO54" s="45">
         <v>9.36</v>
       </c>
       <c r="AP54" s="12"/>
@@ -22326,7 +22453,7 @@
         <v>33.299999999999997</v>
       </c>
       <c r="AN55" s="12"/>
-      <c r="AO55" s="10">
+      <c r="AO55" s="45">
         <v>3.86</v>
       </c>
       <c r="AP55" s="12"/>
@@ -22501,7 +22628,7 @@
         <v>22.38</v>
       </c>
       <c r="AN56" s="12"/>
-      <c r="AO56" s="10">
+      <c r="AO56" s="45">
         <v>3.76</v>
       </c>
       <c r="AP56" s="12"/>
@@ -22672,7 +22799,7 @@
         <v>7.37</v>
       </c>
       <c r="AN57" s="12"/>
-      <c r="AO57" s="10">
+      <c r="AO57" s="45">
         <v>1.91</v>
       </c>
       <c r="AP57" s="12"/>
@@ -22843,7 +22970,7 @@
         <v>19.77</v>
       </c>
       <c r="AN58" s="12"/>
-      <c r="AO58" s="10">
+      <c r="AO58" s="45">
         <v>2.42</v>
       </c>
       <c r="AP58" s="12"/>
@@ -23014,7 +23141,7 @@
         <v>0.83</v>
       </c>
       <c r="AN59" s="12"/>
-      <c r="AO59" s="10">
+      <c r="AO59" s="45">
         <v>0.21</v>
       </c>
       <c r="AP59" s="12"/>
@@ -23183,7 +23310,7 @@
         <v>32</v>
       </c>
       <c r="AN60" s="12"/>
-      <c r="AO60" s="10">
+      <c r="AO60" s="45">
         <v>8.8000000000000007</v>
       </c>
       <c r="AP60" s="12"/>
@@ -23354,7 +23481,7 @@
         <v>59</v>
       </c>
       <c r="AN61" s="12"/>
-      <c r="AO61" s="10">
+      <c r="AO61" s="45">
         <v>6.91</v>
       </c>
       <c r="AP61" s="12"/>
@@ -23523,7 +23650,7 @@
         <v>14.71</v>
       </c>
       <c r="AN62" s="12"/>
-      <c r="AO62" s="10">
+      <c r="AO62" s="45">
         <v>9.9700000000000006</v>
       </c>
       <c r="AP62" s="10">
@@ -23700,7 +23827,7 @@
         <v>32</v>
       </c>
       <c r="AN63" s="12"/>
-      <c r="AO63" s="10">
+      <c r="AO63" s="45">
         <v>4.7</v>
       </c>
       <c r="AP63" s="10">
@@ -23882,14 +24009,14 @@
         <v>7</v>
       </c>
       <c r="AM64" s="10">
-        <v>77.66</v>
+        <v>60.82</v>
       </c>
       <c r="AN64" s="12"/>
-      <c r="AO64" s="10">
-        <v>19.71</v>
-      </c>
-      <c r="AP64" s="10">
-        <v>7.45</v>
+      <c r="AO64" s="47">
+        <v>23.370729999999998</v>
+      </c>
+      <c r="AP64" s="42" t="s">
+        <v>464</v>
       </c>
       <c r="AQ64" s="12"/>
       <c r="AR64" s="12"/>
@@ -23897,14 +24024,14 @@
         <v>7</v>
       </c>
       <c r="AT64" s="10">
-        <v>100</v>
+        <v>63.15</v>
       </c>
       <c r="AU64" s="12"/>
-      <c r="AV64" s="10">
-        <v>25.32</v>
-      </c>
-      <c r="AW64" s="10">
-        <v>9.57</v>
+      <c r="AV64" s="48">
+        <v>32.755009999999999</v>
+      </c>
+      <c r="AW64" s="42" t="s">
+        <v>465</v>
       </c>
       <c r="AX64" s="12"/>
       <c r="AY64" s="12"/>
@@ -23912,14 +24039,14 @@
         <v>7</v>
       </c>
       <c r="BA64" s="10">
-        <v>95.74</v>
+        <v>31.58</v>
       </c>
       <c r="BB64" s="12"/>
-      <c r="BC64" s="10">
-        <v>25.35</v>
-      </c>
-      <c r="BD64" s="10">
-        <v>9.58</v>
+      <c r="BC64" s="42">
+        <v>24.55</v>
+      </c>
+      <c r="BD64" s="42" t="s">
+        <v>466</v>
       </c>
       <c r="BE64" s="12"/>
       <c r="BF64" s="12"/>
@@ -23927,14 +24054,14 @@
         <v>7</v>
       </c>
       <c r="BH64" s="10">
-        <v>104.26</v>
+        <v>35.090000000000003</v>
       </c>
       <c r="BI64" s="12"/>
-      <c r="BJ64" s="10">
-        <v>28.12</v>
-      </c>
-      <c r="BK64" s="10">
-        <v>10.63</v>
+      <c r="BJ64" s="42">
+        <v>25.338000000000001</v>
+      </c>
+      <c r="BK64" s="42" t="s">
+        <v>467</v>
       </c>
       <c r="BL64" s="12"/>
       <c r="BM64" s="12"/>
@@ -24067,14 +24194,14 @@
         <v>7</v>
       </c>
       <c r="AM65" s="10">
-        <v>92.06</v>
+        <v>38.590000000000003</v>
       </c>
       <c r="AN65" s="12"/>
-      <c r="AO65" s="10">
-        <v>33.6</v>
-      </c>
-      <c r="AP65" s="10">
-        <v>12.7</v>
+      <c r="AO65" s="47">
+        <v>31.399249999999999</v>
+      </c>
+      <c r="AP65" s="42" t="s">
+        <v>468</v>
       </c>
       <c r="AQ65" s="12"/>
       <c r="AR65" s="12"/>
@@ -24082,14 +24209,14 @@
         <v>7</v>
       </c>
       <c r="AT65" s="10">
-        <v>92.06</v>
+        <v>50.29</v>
       </c>
       <c r="AU65" s="12"/>
-      <c r="AV65" s="10">
-        <v>11.67</v>
-      </c>
-      <c r="AW65" s="10">
-        <v>4.41</v>
+      <c r="AV65" s="42">
+        <v>23.370729999999998</v>
+      </c>
+      <c r="AW65" s="42" t="s">
+        <v>469</v>
       </c>
       <c r="AX65" s="12"/>
       <c r="AY65" s="12"/>
@@ -24097,14 +24224,14 @@
         <v>7</v>
       </c>
       <c r="BA65" s="10">
-        <v>98.41</v>
+        <v>42.1</v>
       </c>
       <c r="BB65" s="12"/>
-      <c r="BC65" s="10">
-        <v>27.99</v>
-      </c>
-      <c r="BD65" s="10">
-        <v>10.58</v>
+      <c r="BC65" s="42">
+        <v>24.15484</v>
+      </c>
+      <c r="BD65" s="42" t="s">
+        <v>470</v>
       </c>
       <c r="BE65" s="12"/>
       <c r="BF65" s="12"/>
@@ -24112,14 +24239,14 @@
         <v>7</v>
       </c>
       <c r="BH65" s="10">
-        <v>81.48</v>
+        <v>54.97</v>
       </c>
       <c r="BI65" s="12"/>
-      <c r="BJ65" s="10">
-        <v>16.8</v>
-      </c>
-      <c r="BK65" s="10">
-        <v>6.35</v>
+      <c r="BJ65" s="42">
+        <v>25.338000000000001</v>
+      </c>
+      <c r="BK65" s="42" t="s">
+        <v>471</v>
       </c>
       <c r="BL65" s="12"/>
       <c r="BM65" s="12"/>
@@ -24252,14 +24379,14 @@
         <v>7</v>
       </c>
       <c r="AM66" s="10">
-        <v>114.29</v>
+        <v>52.55</v>
       </c>
       <c r="AN66" s="12"/>
-      <c r="AO66" s="10">
-        <v>26.46</v>
-      </c>
-      <c r="AP66" s="10">
-        <v>10</v>
+      <c r="AO66" s="47">
+        <v>47.476860000000002</v>
+      </c>
+      <c r="AP66" s="42" t="s">
+        <v>472</v>
       </c>
       <c r="AQ66" s="12"/>
       <c r="AR66" s="12"/>
@@ -24267,14 +24394,14 @@
         <v>7</v>
       </c>
       <c r="AT66" s="10">
-        <v>82.86</v>
+        <v>92.35</v>
       </c>
       <c r="AU66" s="12"/>
-      <c r="AV66" s="10">
-        <v>18.89</v>
-      </c>
-      <c r="AW66" s="10">
-        <v>7.14</v>
+      <c r="AV66" s="42">
+        <v>36.740319999999997</v>
+      </c>
+      <c r="AW66" s="42" t="s">
+        <v>473</v>
       </c>
       <c r="AX66" s="12"/>
       <c r="AY66" s="12"/>
@@ -24282,14 +24409,14 @@
         <v>7</v>
       </c>
       <c r="BA66" s="10">
-        <v>114.29</v>
+        <v>15.92</v>
       </c>
       <c r="BB66" s="12"/>
-      <c r="BC66" s="10">
-        <v>22.67</v>
-      </c>
-      <c r="BD66" s="10">
-        <v>8.57</v>
+      <c r="BC66" s="42">
+        <v>19.303709999999999</v>
+      </c>
+      <c r="BD66" s="42" t="s">
+        <v>479</v>
       </c>
       <c r="BE66" s="12"/>
       <c r="BF66" s="12"/>
@@ -24297,14 +24424,14 @@
         <v>7</v>
       </c>
       <c r="BH66" s="10">
-        <v>77.14</v>
+        <v>41.4</v>
       </c>
       <c r="BI66" s="12"/>
-      <c r="BJ66" s="10">
-        <v>15.13</v>
-      </c>
-      <c r="BK66" s="10">
-        <v>5.72</v>
+      <c r="BJ66" s="42">
+        <v>19.303709999999999</v>
+      </c>
+      <c r="BK66" s="42" t="s">
+        <v>474</v>
       </c>
       <c r="BL66" s="12"/>
       <c r="BM66" s="12"/>
@@ -24437,14 +24564,14 @@
         <v>7</v>
       </c>
       <c r="AM67" s="10">
-        <v>92.49</v>
+        <v>55.74</v>
       </c>
       <c r="AN67" s="12"/>
-      <c r="AO67" s="10">
-        <v>38.229999999999997</v>
-      </c>
-      <c r="AP67" s="10">
-        <v>14.45</v>
+      <c r="AO67" s="47">
+        <v>55.725009999999997</v>
+      </c>
+      <c r="AP67" s="42" t="s">
+        <v>475</v>
       </c>
       <c r="AQ67" s="12"/>
       <c r="AR67" s="12"/>
@@ -24452,14 +24579,14 @@
         <v>7</v>
       </c>
       <c r="AT67" s="10">
-        <v>63.58</v>
+        <v>41.4</v>
       </c>
       <c r="AU67" s="12"/>
-      <c r="AV67" s="10">
-        <v>15.29</v>
-      </c>
-      <c r="AW67" s="10">
-        <v>5.78</v>
+      <c r="AV67" s="42">
+        <v>29.191009999999999</v>
+      </c>
+      <c r="AW67" s="42" t="s">
+        <v>476</v>
       </c>
       <c r="AX67" s="12"/>
       <c r="AY67" s="12"/>
@@ -24467,14 +24594,14 @@
         <v>7</v>
       </c>
       <c r="BA67" s="10">
-        <v>106.94</v>
+        <v>76.430000000000007</v>
       </c>
       <c r="BB67" s="12"/>
-      <c r="BC67" s="10">
-        <v>38.229999999999997</v>
-      </c>
-      <c r="BD67" s="10">
-        <v>14.45</v>
+      <c r="BC67" s="42">
+        <v>55.72</v>
+      </c>
+      <c r="BD67" s="42" t="s">
+        <v>477</v>
       </c>
       <c r="BE67" s="12"/>
       <c r="BF67" s="12"/>
@@ -24482,14 +24609,14 @@
         <v>7</v>
       </c>
       <c r="BH67" s="10">
-        <v>88.15</v>
+        <v>55.73</v>
       </c>
       <c r="BI67" s="12"/>
-      <c r="BJ67" s="10">
-        <v>15.29</v>
-      </c>
-      <c r="BK67" s="10">
-        <v>5.78</v>
+      <c r="BJ67" s="42">
+        <v>29.191009999999999</v>
+      </c>
+      <c r="BK67" s="42" t="s">
+        <v>478</v>
       </c>
       <c r="BL67" s="12"/>
       <c r="BM67" s="12"/>
@@ -24623,7 +24750,7 @@
         <v>36.67</v>
       </c>
       <c r="AN68" s="12"/>
-      <c r="AO68" s="10">
+      <c r="AO68" s="45">
         <v>16.38</v>
       </c>
       <c r="AP68" s="10">
@@ -24806,7 +24933,7 @@
         <v>23.33</v>
       </c>
       <c r="AN69" s="12"/>
-      <c r="AO69" s="10">
+      <c r="AO69" s="45">
         <v>26.46</v>
       </c>
       <c r="AP69" s="10">
@@ -24989,7 +25116,7 @@
         <v>40.479999999999997</v>
       </c>
       <c r="AN70" s="12"/>
-      <c r="AO70" s="10">
+      <c r="AO70" s="45">
         <v>3.76</v>
       </c>
       <c r="AP70" s="10">
@@ -25172,7 +25299,7 @@
         <v>45.71</v>
       </c>
       <c r="AN71" s="12"/>
-      <c r="AO71" s="10">
+      <c r="AO71" s="45">
         <v>27.73</v>
       </c>
       <c r="AP71" s="10">
@@ -25357,7 +25484,7 @@
         <v>29.64</v>
       </c>
       <c r="AN72" s="12"/>
-      <c r="AO72" s="10">
+      <c r="AO72" s="45">
         <v>19.36</v>
       </c>
       <c r="AP72" s="10">
@@ -25540,7 +25667,7 @@
         <v>34.67</v>
       </c>
       <c r="AN73" s="12"/>
-      <c r="AO73" s="10">
+      <c r="AO73" s="45">
         <v>21.55</v>
       </c>
       <c r="AP73" s="10">
@@ -25719,7 +25846,7 @@
         <v>1</v>
       </c>
       <c r="AN74" s="12"/>
-      <c r="AO74" s="10">
+      <c r="AO74" s="45">
         <v>0.62</v>
       </c>
       <c r="AP74" s="10">
@@ -25900,7 +26027,7 @@
         <v>0.99</v>
       </c>
       <c r="AN75" s="12"/>
-      <c r="AO75" s="10">
+      <c r="AO75" s="45">
         <v>0.66</v>
       </c>
       <c r="AP75" s="10">
@@ -26075,7 +26202,7 @@
         <v>94.71</v>
       </c>
       <c r="AN76" s="12"/>
-      <c r="AO76" s="10">
+      <c r="AO76" s="45">
         <v>4.0199999999999996</v>
       </c>
       <c r="AP76" s="10">
@@ -26250,7 +26377,7 @@
         <v>0.73</v>
       </c>
       <c r="AN77" s="12"/>
-      <c r="AO77" s="10">
+      <c r="AO77" s="45">
         <v>0.11</v>
       </c>
       <c r="AP77" s="10">
@@ -26427,7 +26554,7 @@
         <v>93.78</v>
       </c>
       <c r="AN78" s="12"/>
-      <c r="AO78" s="10">
+      <c r="AO78" s="45">
         <v>5.03</v>
       </c>
       <c r="AP78" s="10">
@@ -26604,7 +26731,7 @@
         <v>92.94</v>
       </c>
       <c r="AN79" s="12"/>
-      <c r="AO79" s="10">
+      <c r="AO79" s="45">
         <v>5.83</v>
       </c>
       <c r="AP79" s="10">
@@ -26781,7 +26908,7 @@
         <v>73.14</v>
       </c>
       <c r="AN80" s="12"/>
-      <c r="AO80" s="10">
+      <c r="AO80" s="45">
         <v>12.93</v>
       </c>
       <c r="AP80" s="10">
@@ -26958,7 +27085,7 @@
         <v>89.06</v>
       </c>
       <c r="AN81" s="12"/>
-      <c r="AO81" s="10">
+      <c r="AO81" s="45">
         <v>5.71</v>
       </c>
       <c r="AP81" s="10">
@@ -27135,7 +27262,7 @@
         <v>90.03</v>
       </c>
       <c r="AN82" s="12"/>
-      <c r="AO82" s="10">
+      <c r="AO82" s="45">
         <v>4.05</v>
       </c>
       <c r="AP82" s="10">
@@ -27312,7 +27439,7 @@
         <v>0.44</v>
       </c>
       <c r="AN83" s="12"/>
-      <c r="AO83" s="10">
+      <c r="AO83" s="45">
         <v>0.24</v>
       </c>
       <c r="AP83" s="10">
@@ -27487,7 +27614,7 @@
         <v>83.39</v>
       </c>
       <c r="AN84" s="12"/>
-      <c r="AO84" s="10">
+      <c r="AO84" s="45">
         <v>7.66</v>
       </c>
       <c r="AP84" s="10">
@@ -27662,7 +27789,7 @@
         <v>1.02</v>
       </c>
       <c r="AN85" s="12"/>
-      <c r="AO85" s="10">
+      <c r="AO85" s="45">
         <v>0.66</v>
       </c>
       <c r="AP85" s="10">
@@ -27841,7 +27968,7 @@
         <v>74.14</v>
       </c>
       <c r="AN86" s="12"/>
-      <c r="AO86" s="10">
+      <c r="AO86" s="45">
         <v>10.85</v>
       </c>
       <c r="AP86" s="10">
@@ -28018,7 +28145,7 @@
         <v>266.92</v>
       </c>
       <c r="AN87" s="12"/>
-      <c r="AO87" s="10">
+      <c r="AO87" s="45">
         <v>192.46</v>
       </c>
       <c r="AP87" s="10">
@@ -28195,7 +28322,7 @@
         <v>303.06</v>
       </c>
       <c r="AN88" s="12"/>
-      <c r="AO88" s="10">
+      <c r="AO88" s="45">
         <v>66.69</v>
       </c>
       <c r="AP88" s="10">
@@ -28372,7 +28499,7 @@
         <v>0.06</v>
       </c>
       <c r="AN89" s="12"/>
-      <c r="AO89" s="10">
+      <c r="AO89" s="45">
         <v>0.09</v>
       </c>
       <c r="AP89" s="10">
@@ -28553,7 +28680,7 @@
         <v>62.66</v>
       </c>
       <c r="AN90" s="12"/>
-      <c r="AO90" s="10">
+      <c r="AO90" s="45">
         <v>11.81</v>
       </c>
       <c r="AP90" s="10">
@@ -28736,7 +28863,7 @@
         <v>35.909999999999997</v>
       </c>
       <c r="AN91" s="12"/>
-      <c r="AO91" s="10">
+      <c r="AO91" s="45">
         <v>9.4600000000000009</v>
       </c>
       <c r="AP91" s="10">
@@ -28915,7 +29042,7 @@
         <v>66.14</v>
       </c>
       <c r="AN92" s="12"/>
-      <c r="AO92" s="10">
+      <c r="AO92" s="45">
         <v>6.37</v>
       </c>
       <c r="AP92" s="10">
@@ -29088,7 +29215,7 @@
         <v>4.2300000000000004</v>
       </c>
       <c r="AN93" s="12"/>
-      <c r="AO93" s="10">
+      <c r="AO93" s="45">
         <v>0.73</v>
       </c>
       <c r="AP93" s="10">
@@ -29261,7 +29388,7 @@
         <v>2.5099999999999998</v>
       </c>
       <c r="AN94" s="12"/>
-      <c r="AO94" s="10">
+      <c r="AO94" s="45">
         <v>0.48</v>
       </c>
       <c r="AP94" s="10">
@@ -29433,14 +29560,14 @@
         <v>4</v>
       </c>
       <c r="AM95" s="10">
-        <v>49.86</v>
+        <v>22.2</v>
       </c>
       <c r="AN95" s="12"/>
-      <c r="AO95" s="10">
-        <v>17</v>
-      </c>
-      <c r="AP95" s="10">
-        <v>8.5</v>
+      <c r="AO95" s="47">
+        <v>19.05247</v>
+      </c>
+      <c r="AP95" s="42" t="s">
+        <v>480</v>
       </c>
       <c r="AQ95" s="12"/>
       <c r="AR95" s="12"/>
@@ -29448,14 +29575,14 @@
         <v>4</v>
       </c>
       <c r="AT95" s="10">
-        <v>69.569999999999993</v>
+        <v>47.09</v>
       </c>
       <c r="AU95" s="12"/>
-      <c r="AV95" s="10">
-        <v>22.42</v>
-      </c>
-      <c r="AW95" s="10">
-        <v>11.21</v>
+      <c r="AV95" s="42">
+        <v>30.8322</v>
+      </c>
+      <c r="AW95" s="42" t="s">
+        <v>481</v>
       </c>
       <c r="AX95" s="12"/>
       <c r="AY95" s="12"/>
@@ -29463,14 +29590,14 @@
         <v>4</v>
       </c>
       <c r="BA95" s="10">
-        <v>77.290000000000006</v>
+        <v>1.91</v>
       </c>
       <c r="BB95" s="12"/>
-      <c r="BC95" s="10">
-        <v>24.74</v>
-      </c>
-      <c r="BD95" s="10">
-        <v>12.37</v>
+      <c r="BC95" s="42">
+        <v>23.12236</v>
+      </c>
+      <c r="BD95" s="42" t="s">
+        <v>482</v>
       </c>
       <c r="BE95" s="12"/>
       <c r="BF95" s="12"/>
@@ -29478,14 +29605,14 @@
         <v>4</v>
       </c>
       <c r="BH95" s="10">
-        <v>62.22</v>
+        <v>17.23</v>
       </c>
       <c r="BI95" s="12"/>
-      <c r="BJ95" s="10">
-        <v>18.559999999999999</v>
-      </c>
-      <c r="BK95" s="10">
-        <v>9.2799999999999994</v>
+      <c r="BJ95" s="42">
+        <v>18.099930000000001</v>
+      </c>
+      <c r="BK95" s="42" t="s">
+        <v>483</v>
       </c>
       <c r="BL95" s="12"/>
       <c r="BM95" s="12"/>
@@ -29617,7 +29744,7 @@
         <v>39.78</v>
       </c>
       <c r="AN96" s="12"/>
-      <c r="AO96" s="10">
+      <c r="AO96" s="45">
         <v>21.164585989999999</v>
       </c>
       <c r="AP96" s="10">
@@ -29803,14 +29930,14 @@
         <v>13</v>
       </c>
       <c r="AM97" s="10">
-        <v>15.24</v>
+        <v>4.03</v>
       </c>
       <c r="AN97" s="12"/>
-      <c r="AO97" s="10">
-        <v>3.6416067879999998</v>
-      </c>
-      <c r="AP97" s="10">
-        <v>1.01</v>
+      <c r="AO97" s="47">
+        <v>5.4679710000000004</v>
+      </c>
+      <c r="AP97" s="42" t="s">
+        <v>484</v>
       </c>
       <c r="AQ97" s="12"/>
       <c r="AR97" s="12"/>
@@ -29818,14 +29945,14 @@
         <v>11</v>
       </c>
       <c r="AT97" s="10">
-        <v>10.86</v>
+        <v>7.08</v>
       </c>
       <c r="AU97" s="12"/>
-      <c r="AV97" s="10">
-        <v>3.3497910380000002</v>
-      </c>
-      <c r="AW97" s="10">
-        <v>1.01</v>
+      <c r="AV97" s="42">
+        <v>6.5005850000000001</v>
+      </c>
+      <c r="AW97" s="42" t="s">
+        <v>487</v>
       </c>
       <c r="AX97" s="12"/>
       <c r="AY97" s="12"/>
@@ -29833,14 +29960,14 @@
         <v>11</v>
       </c>
       <c r="BA97" s="10">
-        <v>11.54</v>
+        <v>5.53</v>
       </c>
       <c r="BB97" s="12"/>
-      <c r="BC97" s="10">
-        <v>4.178947236</v>
-      </c>
-      <c r="BD97" s="10">
-        <v>1.26</v>
+      <c r="BC97" s="42">
+        <v>5.5250430000000001</v>
+      </c>
+      <c r="BD97" s="42" t="s">
+        <v>485</v>
       </c>
       <c r="BE97" s="12"/>
       <c r="BF97" s="12"/>
@@ -29848,14 +29975,14 @@
         <v>10</v>
       </c>
       <c r="BH97" s="10">
-        <v>10.69</v>
+        <v>4.7699999999999996</v>
       </c>
       <c r="BI97" s="12"/>
-      <c r="BJ97" s="10">
-        <v>4.016092628</v>
-      </c>
-      <c r="BK97" s="10">
-        <v>1.27</v>
+      <c r="BJ97" s="42">
+        <v>7.0938699999999999</v>
+      </c>
+      <c r="BK97" s="42" t="s">
+        <v>486</v>
       </c>
       <c r="BL97" s="12"/>
       <c r="BM97" s="12"/>

</xml_diff>